<commit_message>
Exchange Parent, Child columns
</commit_message>
<xml_diff>
--- a/Parent-Child_list.xlsx
+++ b/Parent-Child_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11122"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryozo/Downloads/dxf_diff_results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ryozo/Dropbox/Client/ULVAC/ElectricDesignManagement/ReuseSystem/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED4EB82-7B00-0943-A3DF-51A6E38D85F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8007E0CD-C69C-954A-B12F-33E65568D5C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="620" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8420" yWindow="5800" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
   <si>
     <t>Parent</t>
   </si>
@@ -43,30 +43,48 @@
     <t>Note</t>
   </si>
   <si>
-    <t>Total Entties</t>
+    <t>Deleted Entities</t>
+  </si>
+  <si>
+    <t>Added Entities</t>
   </si>
   <si>
     <t>Diff Entities</t>
   </si>
   <si>
+    <t>Unchanged Entities</t>
+  </si>
+  <si>
+    <t>Total Entities</t>
+  </si>
+  <si>
+    <t>EE6666-365-61A</t>
+  </si>
+  <si>
+    <t>EE6333-610-07A</t>
+  </si>
+  <si>
+    <t>EE6333-365-61B</t>
+  </si>
+  <si>
+    <t>EE6331-370-51A</t>
+  </si>
+  <si>
+    <t>EE5611-695-04B</t>
+  </si>
+  <si>
+    <t>EE6097-039-06C</t>
+  </si>
+  <si>
+    <t>EE6333-610-07B</t>
+  </si>
+  <si>
+    <t>EE6666-365-61B</t>
+  </si>
+  <si>
     <t>EE6333-365-61C</t>
   </si>
   <si>
-    <t>EE6106-370-51B</t>
-  </si>
-  <si>
-    <t>EE5611-695-04B</t>
-  </si>
-  <si>
-    <t>EE6097-039-06C</t>
-  </si>
-  <si>
-    <t>EE6333-610-07B</t>
-  </si>
-  <si>
-    <t>EE6666-365-61B</t>
-  </si>
-  <si>
     <t>EE6331-370-51B</t>
   </si>
   <si>
@@ -79,22 +97,31 @@
     <t>EE6666-610-05A</t>
   </si>
   <si>
+    <t>RevUp</t>
+  </si>
+  <si>
     <t>流用</t>
   </si>
   <si>
     <t>PROCESS_POWER_SUPPLY_R1</t>
   </si>
   <si>
+    <t>ELECTRICAL SCHEMATIC DIAGRAM</t>
+  </si>
+  <si>
+    <t>PROCESS_POWER_SUPPLY_R3</t>
+  </si>
+  <si>
     <t>ＭＯＴＯＲ（Ｔ/Ｍ）　Ｒ１</t>
   </si>
   <si>
-    <t>ELECTRICAL SCHEMATIC DIAGRAM</t>
-  </si>
-  <si>
     <t>ＵＮＩＴ内結線図</t>
   </si>
   <si>
     <t>ケ－ブル一覧表</t>
+  </si>
+  <si>
+    <t>ＰＲＯＣＥＳＳ　ＰＯＷＥＲ　ＳＵＰＰＬＹ１ Ｒ３</t>
   </si>
   <si>
     <t>ＭＡＧＮＥＴ　ＵＰ／ＤＯＷＮ　Ｒ１</t>
@@ -482,30 +509,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
-  <cols>
-    <col min="1" max="2" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -528,105 +545,259 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="2">
+        <v>45993.155399224437</v>
+      </c>
+      <c r="H2">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="I2">
+        <v>6</v>
+      </c>
+      <c r="J2">
+        <v>15</v>
+      </c>
+      <c r="K2">
+        <v>614</v>
+      </c>
+      <c r="L2">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="2">
+        <v>45993.155399257121</v>
+      </c>
+      <c r="H3">
+        <v>26</v>
+      </c>
+      <c r="I3">
+        <v>7</v>
+      </c>
+      <c r="J3">
+        <v>33</v>
+      </c>
+      <c r="K3">
+        <v>6620</v>
+      </c>
+      <c r="L3">
+        <v>6653</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="C4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="2">
+        <v>45993.155399283969</v>
+      </c>
+      <c r="H4">
+        <v>35</v>
+      </c>
+      <c r="I4">
+        <v>13</v>
+      </c>
+      <c r="J4">
+        <v>48</v>
+      </c>
+      <c r="K4">
+        <v>598</v>
+      </c>
+      <c r="L4">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="2">
+        <v>45993.155399308227</v>
+      </c>
+      <c r="H5">
+        <v>12</v>
+      </c>
+      <c r="I5">
+        <v>6</v>
+      </c>
+      <c r="J5">
+        <v>18</v>
+      </c>
+      <c r="K5">
+        <v>563</v>
+      </c>
+      <c r="L5">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="2">
+        <v>45993.155399332143</v>
+      </c>
+      <c r="H6">
+        <v>11</v>
+      </c>
+      <c r="I6">
+        <v>15</v>
+      </c>
+      <c r="J6">
+        <v>26</v>
+      </c>
+      <c r="K6">
+        <v>3496</v>
+      </c>
+      <c r="L6">
+        <v>3522</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="2">
+        <v>45993.155399355761</v>
+      </c>
+      <c r="H7">
+        <v>33</v>
+      </c>
+      <c r="I7">
+        <v>59</v>
+      </c>
+      <c r="J7">
+        <v>92</v>
+      </c>
+      <c r="K7">
+        <v>2861</v>
+      </c>
+      <c r="L7">
+        <v>2953</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="2">
-        <v>45992.054740633037</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="2">
-        <v>45992.054740642372</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="2">
-        <v>45992.054740646578</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="B8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="2">
-        <v>45992.054740650317</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="2">
-        <v>45992.054740654123</v>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="2">
+        <v>45993.155399382536</v>
+      </c>
+      <c r="H8">
+        <v>60</v>
+      </c>
+      <c r="I8">
+        <v>58</v>
+      </c>
+      <c r="J8">
+        <v>118</v>
+      </c>
+      <c r="K8">
+        <v>6588</v>
+      </c>
+      <c r="L8">
+        <v>6706</v>
       </c>
     </row>
   </sheetData>

</xml_diff>